<commit_message>
Nuevas variables de entrada.
</commit_message>
<xml_diff>
--- a/Variables de entrada.xlsx
+++ b/Variables de entrada.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="10335" windowHeight="4965"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="10335" windowHeight="4965" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="423">
   <si>
     <t>Descripción</t>
   </si>
@@ -568,6 +568,723 @@
   </si>
   <si>
     <t>diam_feed_neg</t>
+  </si>
+  <si>
+    <t>Función</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>Long (Byref)</t>
+  </si>
+  <si>
+    <t>Contador global de fila de la hoja de replanteo</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Contador global de fila de puntos singulares</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>Contador global de fila de trazado</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Contador local de fila de hoja de replanteo</t>
+  </si>
+  <si>
+    <t>pk0</t>
+  </si>
+  <si>
+    <t>Double</t>
+  </si>
+  <si>
+    <t>Pk actual</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>Contador global de columnas de puntos singulares</t>
+  </si>
+  <si>
+    <t>Nombre NUEVO</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>pk1</t>
+  </si>
+  <si>
+    <t>Pk del poste a ubicar antes del PS</t>
+  </si>
+  <si>
+    <t>pk2</t>
+  </si>
+  <si>
+    <t>Pk del poste a ubicar después del PS</t>
+  </si>
+  <si>
+    <t>div</t>
+  </si>
+  <si>
+    <t>Resto de la división de dist entre inc_va</t>
+  </si>
+  <si>
+    <t>vano12</t>
+  </si>
+  <si>
+    <t>Vano entre pk1 y pk2</t>
+  </si>
+  <si>
+    <t>vanoref</t>
+  </si>
+  <si>
+    <t>Parte divisible por inc_va</t>
+  </si>
+  <si>
+    <t>l1</t>
+  </si>
+  <si>
+    <t>Distancia entre inicio de paso superior y pk (actual-1)</t>
+  </si>
+  <si>
+    <t>l2</t>
+  </si>
+  <si>
+    <t>Distancia entre pk actual y final de paso superior</t>
+  </si>
+  <si>
+    <t>vano0</t>
+  </si>
+  <si>
+    <t>Vano actual</t>
+  </si>
+  <si>
+    <t>dist_restar</t>
+  </si>
+  <si>
+    <t>Longitud a corregir entre poste actual y poste futuro</t>
+  </si>
+  <si>
+    <t>pmedio</t>
+  </si>
+  <si>
+    <t>Punto medio (Vano actual – longitud paso superior)</t>
+  </si>
+  <si>
+    <t>Contador global de columna de puntos singulares</t>
+  </si>
+  <si>
+    <t>vano01</t>
+  </si>
+  <si>
+    <t>Vano entre pk1 y pk0</t>
+  </si>
+  <si>
+    <t>pkref</t>
+  </si>
+  <si>
+    <t>Pk (actual +1)</t>
+  </si>
+  <si>
+    <t>Pk (actual)</t>
+  </si>
+  <si>
+    <t>Pk del poste a ubicar en la primera pila del viaducto</t>
+  </si>
+  <si>
+    <t>Pk del poste a ubicar en la siguiente pila o fuera de viaducto</t>
+  </si>
+  <si>
+    <t>Vano para caso particular de tener un PS antes de la aguja</t>
+  </si>
+  <si>
+    <t>Pk del poste a ubicar en la aguja</t>
+  </si>
+  <si>
+    <t>Longitud de la clotoide de entrada</t>
+  </si>
+  <si>
+    <t>Longitud de la clotoide de salida</t>
+  </si>
+  <si>
+    <t>rady</t>
+  </si>
+  <si>
+    <t>Radio de la curva</t>
+  </si>
+  <si>
+    <t>rady2</t>
+  </si>
+  <si>
+    <t>Radio de la curva anterior</t>
+  </si>
+  <si>
+    <t>inicio1</t>
+  </si>
+  <si>
+    <t>Pk de inicio de la clotoide de entrada</t>
+  </si>
+  <si>
+    <t>inicio2</t>
+  </si>
+  <si>
+    <t>Pk de inicio de la clotoide de salida</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>Parámetro de la clotoide de entrada</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>Parámetro de la clotoide de entrada de la curva siguiente</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>Parámetro de la clotoide de salida</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Coeficiente de confort</t>
+  </si>
+  <si>
+    <t>final</t>
+  </si>
+  <si>
+    <t>Pk inicio de la curva siguiente</t>
+  </si>
+  <si>
+    <t>radioC</t>
+  </si>
+  <si>
+    <t>Radio del tramo de clotoide en el primer bucle</t>
+  </si>
+  <si>
+    <t>radioC1</t>
+  </si>
+  <si>
+    <t>Radio del tramo de clotoide en el segundo bucle</t>
+  </si>
+  <si>
+    <t>radioC2</t>
+  </si>
+  <si>
+    <t>contador</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Contador de doble bucle</t>
+  </si>
+  <si>
+    <t>dev</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>Peralte</t>
+  </si>
+  <si>
+    <t>z_sing1</t>
+  </si>
+  <si>
+    <t>z_ps</t>
+  </si>
+  <si>
+    <t>div_ps</t>
+  </si>
+  <si>
+    <t>pk_1_ps</t>
+  </si>
+  <si>
+    <t>va_ref_ps</t>
+  </si>
+  <si>
+    <t>l_1_ps</t>
+  </si>
+  <si>
+    <t>va_0_ps</t>
+  </si>
+  <si>
+    <t>dist_restar_ps</t>
+  </si>
+  <si>
+    <t>pto_medio_ps</t>
+  </si>
+  <si>
+    <t>pk_0_ps</t>
+  </si>
+  <si>
+    <t>l_0_ps</t>
+  </si>
+  <si>
+    <t>va_2_ps</t>
+  </si>
+  <si>
+    <t>rayon</t>
+  </si>
+  <si>
+    <t>Double (Byref)</t>
+  </si>
+  <si>
+    <t>Radio actual</t>
+  </si>
+  <si>
+    <t>Contador local de fila de tabla de radios-vanos-descentramientos</t>
+  </si>
+  <si>
+    <t>Vano</t>
+  </si>
+  <si>
+    <t>Vano que se corresponde con el radio</t>
+  </si>
+  <si>
+    <t>Contador local de fila de la hoja de replanteo</t>
+  </si>
+  <si>
+    <t>aloc</t>
+  </si>
+  <si>
+    <t>Contador local de fila de puntos singulares</t>
+  </si>
+  <si>
+    <t>valor</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Texto del comentario</t>
+  </si>
+  <si>
+    <t>guardar</t>
+  </si>
+  <si>
+    <t>Texto a añadir en celdas compartidas</t>
+  </si>
+  <si>
+    <t>descentramiento</t>
+  </si>
+  <si>
+    <t>Descentramiento que se corresponde con el radio</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Contador local auxiliar de fila de hoja de replanteo</t>
+  </si>
+  <si>
+    <t>Amx</t>
+  </si>
+  <si>
+    <t>Altura del hilo de contacto (tramos centrales)</t>
+  </si>
+  <si>
+    <t>Amx1</t>
+  </si>
+  <si>
+    <t>Altura del hilo de contacto (tramos iniciales y finales)</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>Contador de postes para cada PK</t>
+  </si>
+  <si>
+    <t>bis</t>
+  </si>
+  <si>
+    <t>Contador de postes para PK bis</t>
+  </si>
+  <si>
+    <t>kloc</t>
+  </si>
+  <si>
+    <t>Contador local de fila de trazado</t>
+  </si>
+  <si>
+    <t>bloc</t>
+  </si>
+  <si>
+    <t>Contador local de columna de puntos singulares</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Contador de comentarios</t>
+  </si>
+  <si>
+    <t>Pk actual + 1</t>
+  </si>
+  <si>
+    <t>vano1</t>
+  </si>
+  <si>
+    <t>Vano actual + 1</t>
+  </si>
+  <si>
+    <t>vanox</t>
+  </si>
+  <si>
+    <t>Vano correspondiente al radio actual</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>pk_0_sing1</t>
+  </si>
+  <si>
+    <t>sing1 (sing1)</t>
+  </si>
+  <si>
+    <t>sing (sing0)</t>
+  </si>
+  <si>
+    <t>PS (ps)</t>
+  </si>
+  <si>
+    <t>viaduc (viad)</t>
+  </si>
+  <si>
+    <t>aguja (ag)</t>
+  </si>
+  <si>
+    <t>radio (r0)</t>
+  </si>
+  <si>
+    <t>radio1 (r1)</t>
+  </si>
+  <si>
+    <t>vano (va)</t>
+  </si>
+  <si>
+    <t>Regulación (reg)</t>
+  </si>
+  <si>
+    <t>comentarios (com)</t>
+  </si>
+  <si>
+    <t>des (d)</t>
+  </si>
+  <si>
+    <t>altura (alt)</t>
+  </si>
+  <si>
+    <t>postes (poste)</t>
+  </si>
+  <si>
+    <t>revision (rev)</t>
+  </si>
+  <si>
+    <t>z_viad</t>
+  </si>
+  <si>
+    <t>va_0_viad</t>
+  </si>
+  <si>
+    <t>va_1_viad</t>
+  </si>
+  <si>
+    <t>va_2_viad</t>
+  </si>
+  <si>
+    <t>pk_1_viad</t>
+  </si>
+  <si>
+    <t>pk_0_viad</t>
+  </si>
+  <si>
+    <t>pk_0_pila_viad</t>
+  </si>
+  <si>
+    <t>pk_1_pila_viad</t>
+  </si>
+  <si>
+    <t>dist_restar_viad</t>
+  </si>
+  <si>
+    <t>va_ref_ag</t>
+  </si>
+  <si>
+    <t>va_2_ag</t>
+  </si>
+  <si>
+    <t>pk_0_ag</t>
+  </si>
+  <si>
+    <t>pk_1_ag</t>
+  </si>
+  <si>
+    <t>dist_restar_ag</t>
+  </si>
+  <si>
+    <t>l_clot_0_r0</t>
+  </si>
+  <si>
+    <t>l_clot_1_r0</t>
+  </si>
+  <si>
+    <t>r_1_r0</t>
+  </si>
+  <si>
+    <t>r_0_r0</t>
+  </si>
+  <si>
+    <t>pk_clot_0_r0</t>
+  </si>
+  <si>
+    <t>pk_clot_1_r0</t>
+  </si>
+  <si>
+    <t>par_clot_0_r0</t>
+  </si>
+  <si>
+    <t>par_clot_1_r0</t>
+  </si>
+  <si>
+    <t>par_clot_2_r0</t>
+  </si>
+  <si>
+    <t>c_r0</t>
+  </si>
+  <si>
+    <t>pk_1_r0</t>
+  </si>
+  <si>
+    <t>r_clot_0_r0</t>
+  </si>
+  <si>
+    <t>r_clot_1_r0</t>
+  </si>
+  <si>
+    <t>r_clot_2_r0</t>
+  </si>
+  <si>
+    <t>pk_0_r0</t>
+  </si>
+  <si>
+    <t>per_r0</t>
+  </si>
+  <si>
+    <t>r_1_r1</t>
+  </si>
+  <si>
+    <t>r_0_r1</t>
+  </si>
+  <si>
+    <t>pk_clot_0_r1</t>
+  </si>
+  <si>
+    <t>pk_clot_1_r1</t>
+  </si>
+  <si>
+    <t>par_clot_0_r1</t>
+  </si>
+  <si>
+    <t>par_clot_1_r1</t>
+  </si>
+  <si>
+    <t>par_clot_2_r1</t>
+  </si>
+  <si>
+    <t>c_r1</t>
+  </si>
+  <si>
+    <t>pk_1_r1</t>
+  </si>
+  <si>
+    <t>r_clot_0_r1</t>
+  </si>
+  <si>
+    <t>r_clot_1_r1</t>
+  </si>
+  <si>
+    <t>r_clot_2_r1</t>
+  </si>
+  <si>
+    <t>pk_0_r1</t>
+  </si>
+  <si>
+    <t>per_r1</t>
+  </si>
+  <si>
+    <t>l_1_r1</t>
+  </si>
+  <si>
+    <t>l_0_r1</t>
+  </si>
+  <si>
+    <t>m_va</t>
+  </si>
+  <si>
+    <t>va_va</t>
+  </si>
+  <si>
+    <t>z_com</t>
+  </si>
+  <si>
+    <t>q_com</t>
+  </si>
+  <si>
+    <t>val_com</t>
+  </si>
+  <si>
+    <t>guardar_com</t>
+  </si>
+  <si>
+    <t>z_d</t>
+  </si>
+  <si>
+    <t>m_d</t>
+  </si>
+  <si>
+    <t>d_0_d</t>
+  </si>
+  <si>
+    <t>r_0_d</t>
+  </si>
+  <si>
+    <t>z_alt</t>
+  </si>
+  <si>
+    <t>q_alt</t>
+  </si>
+  <si>
+    <t>s_alt</t>
+  </si>
+  <si>
+    <t>alt_hc_tc_alt</t>
+  </si>
+  <si>
+    <t>alt_hc_tif_alt</t>
+  </si>
+  <si>
+    <t>z_poste</t>
+  </si>
+  <si>
+    <t>w_poste</t>
+  </si>
+  <si>
+    <t>bis_poste</t>
+  </si>
+  <si>
+    <t>alt_hc_tc_poste</t>
+  </si>
+  <si>
+    <t>alt_hc_tif_poste</t>
+  </si>
+  <si>
+    <t>z_rev</t>
+  </si>
+  <si>
+    <t>q_rev</t>
+  </si>
+  <si>
+    <t>k_rev</t>
+  </si>
+  <si>
+    <t>b_rev</t>
+  </si>
+  <si>
+    <t>r_1_rev</t>
+  </si>
+  <si>
+    <t>r_0_rev</t>
+  </si>
+  <si>
+    <t>pk_clot_0_rev</t>
+  </si>
+  <si>
+    <t>pk_clot_1_rev</t>
+  </si>
+  <si>
+    <t>par_clot_0_rev</t>
+  </si>
+  <si>
+    <t>par_clot_1_rev</t>
+  </si>
+  <si>
+    <t>par_clot_2_rev</t>
+  </si>
+  <si>
+    <t>c_rev</t>
+  </si>
+  <si>
+    <t>pk_1_rev</t>
+  </si>
+  <si>
+    <t>r_clot_0_rev</t>
+  </si>
+  <si>
+    <t>r_clot_1_rev</t>
+  </si>
+  <si>
+    <t>r_clot_2_rev</t>
+  </si>
+  <si>
+    <t>cont_rev</t>
+  </si>
+  <si>
+    <t>pk_0_rev</t>
+  </si>
+  <si>
+    <t>per_rev</t>
+  </si>
+  <si>
+    <t>va_0_rev</t>
+  </si>
+  <si>
+    <t>va_1_rev</t>
+  </si>
+  <si>
+    <t>va_r_1_rev</t>
+  </si>
+  <si>
+    <t>l_0_rev</t>
+  </si>
+  <si>
+    <t>l_1_rev</t>
+  </si>
+  <si>
+    <t>g_rev</t>
+  </si>
+  <si>
+    <t>y_r0</t>
+  </si>
+  <si>
+    <t>y_r1</t>
   </si>
 </sst>
 </file>
@@ -604,7 +1321,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -623,17 +1340,112 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -938,8 +1750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -951,7 +1763,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1910,13 +2722,2346 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="10" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E25" s="8"/>
+      <c r="F25" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="4"/>
+      <c r="B26" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E26" s="8"/>
+      <c r="F26" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
+      <c r="B27" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E27" s="8"/>
+      <c r="F27" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+      <c r="B28" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="4"/>
+      <c r="B29" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="4"/>
+      <c r="B30" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="4"/>
+      <c r="B31" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="4"/>
+      <c r="B32" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="4"/>
+      <c r="B33" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="4"/>
+      <c r="B34" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="4"/>
+      <c r="B35" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="4"/>
+      <c r="B36" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="4"/>
+      <c r="B37" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E38" s="8"/>
+      <c r="F38" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="4"/>
+      <c r="B39" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E39" s="8"/>
+      <c r="F39" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="4"/>
+      <c r="B40" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E40" s="8"/>
+      <c r="F40" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="4"/>
+      <c r="B41" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E41" s="8"/>
+      <c r="F41" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="4"/>
+      <c r="B42" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="4"/>
+      <c r="B43" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="4"/>
+      <c r="B44" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="4"/>
+      <c r="B45" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="4"/>
+      <c r="B46" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E47" s="8"/>
+      <c r="F47" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="4"/>
+      <c r="B48" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E48" s="8"/>
+      <c r="F48" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="4"/>
+      <c r="B49" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="4"/>
+      <c r="B50" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="4"/>
+      <c r="B51" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="4"/>
+      <c r="B52" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="4"/>
+      <c r="B53" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="4"/>
+      <c r="B54" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="4"/>
+      <c r="B55" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="D55" s="6"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="4"/>
+      <c r="B56" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="D56" s="6"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="6" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="4"/>
+      <c r="B57" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="D57" s="6"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="6" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="4"/>
+      <c r="B58" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="D58" s="6"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="4"/>
+      <c r="B59" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="D59" s="6"/>
+      <c r="E59" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="4"/>
+      <c r="B60" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="D60" s="6"/>
+      <c r="E60" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="4"/>
+      <c r="B61" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="D61" s="6"/>
+      <c r="E61" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="4"/>
+      <c r="B62" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="D62" s="6"/>
+      <c r="E62" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="4"/>
+      <c r="B63" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="E63" s="8"/>
+      <c r="F63" s="6" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="4"/>
+      <c r="B64" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="4"/>
+      <c r="B65" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E66" s="8"/>
+      <c r="F66" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="4"/>
+      <c r="B67" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E67" s="8"/>
+      <c r="F67" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="4"/>
+      <c r="B68" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="4"/>
+      <c r="B69" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E69" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="4"/>
+      <c r="B70" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E70" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="4"/>
+      <c r="B71" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E71" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="4"/>
+      <c r="B72" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E72" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="4"/>
+      <c r="B73" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E73" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="4"/>
+      <c r="B74" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E74" s="8"/>
+      <c r="F74" s="6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="4"/>
+      <c r="B75" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E75" s="8"/>
+      <c r="F75" s="6" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="4"/>
+      <c r="B76" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E76" s="8"/>
+      <c r="F76" s="6" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="4"/>
+      <c r="B77" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E77" s="8"/>
+      <c r="F77" s="6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="4"/>
+      <c r="B78" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E78" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="4"/>
+      <c r="B79" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E79" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="4"/>
+      <c r="B80" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E80" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="4"/>
+      <c r="B81" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E81" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="4"/>
+      <c r="B82" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="E82" s="8"/>
+      <c r="F82" s="6" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="4"/>
+      <c r="B83" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E83" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="4"/>
+      <c r="B84" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E84" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="E85" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="4"/>
+      <c r="B86" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="E86" s="8"/>
+      <c r="F86" s="6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="4"/>
+      <c r="B87" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E87" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E88" s="8"/>
+      <c r="F88" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="4"/>
+      <c r="B89" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E89" s="8"/>
+      <c r="F89" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="4"/>
+      <c r="B90" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E90" s="8"/>
+      <c r="F90" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="D91" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E91" s="8"/>
+      <c r="F91" s="6" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="4"/>
+      <c r="B92" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E92" s="8"/>
+      <c r="F92" s="6" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" s="4"/>
+      <c r="B93" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="E93" s="8"/>
+      <c r="F93" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" s="4"/>
+      <c r="B94" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="D94" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="E94" s="8"/>
+      <c r="F94" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="D95" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E95" s="8"/>
+      <c r="F95" s="6" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" s="4"/>
+      <c r="B96" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="D96" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E96" s="8"/>
+      <c r="F96" s="6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" s="4"/>
+      <c r="B97" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="D97" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E97" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F97" s="6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" s="4"/>
+      <c r="B98" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="D98" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E98" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F98" s="6" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="D99" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E99" s="8"/>
+      <c r="F99" s="6" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" s="4"/>
+      <c r="B100" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="D100" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E100" s="8"/>
+      <c r="F100" s="6" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" s="4"/>
+      <c r="B101" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="D101" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E101" s="8"/>
+      <c r="F101" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" s="4"/>
+      <c r="B102" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="D102" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E102" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="F102" s="6" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" s="4"/>
+      <c r="B103" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="D103" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E103" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="F103" s="6" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="D104" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E104" s="8"/>
+      <c r="F104" s="6" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105" s="4"/>
+      <c r="B105" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="E105" s="8"/>
+      <c r="F105" s="6" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106" s="4"/>
+      <c r="B106" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="D106" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="E106" s="8"/>
+      <c r="F106" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A107" s="4"/>
+      <c r="B107" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="D107" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E107" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="F107" s="6" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A108" s="4"/>
+      <c r="B108" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="D108" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E108" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="F108" s="6" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A109" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="D109" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E109" s="8"/>
+      <c r="F109" s="6" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A110" s="4"/>
+      <c r="B110" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="D110" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E110" s="8"/>
+      <c r="F110" s="6" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A111" s="4"/>
+      <c r="B111" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E111" s="8"/>
+      <c r="F111" s="6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A112" s="4"/>
+      <c r="B112" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="D112" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E112" s="8"/>
+      <c r="F112" s="6" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A113" s="4"/>
+      <c r="B113" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E113" s="8"/>
+      <c r="F113" s="6" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A114" s="4"/>
+      <c r="B114" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="D114" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E114" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F114" s="6" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A115" s="4"/>
+      <c r="B115" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="D115" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E115" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F115" s="6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A116" s="4"/>
+      <c r="B116" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="C116" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="D116" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E116" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F116" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A117" s="4"/>
+      <c r="B117" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C117" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="D117" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E117" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F117" s="6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A118" s="4"/>
+      <c r="B118" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="C118" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="D118" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E118" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F118" s="6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A119" s="4"/>
+      <c r="B119" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C119" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="D119" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E119" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F119" s="6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A120" s="4"/>
+      <c r="B120" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C120" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="D120" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E120" s="8"/>
+      <c r="F120" s="6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A121" s="4"/>
+      <c r="B121" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C121" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="D121" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E121" s="8"/>
+      <c r="F121" s="6" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A122" s="4"/>
+      <c r="B122" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C122" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="D122" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E122" s="8"/>
+      <c r="F122" s="6" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A123" s="4"/>
+      <c r="B123" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C123" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="D123" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E123" s="8"/>
+      <c r="F123" s="6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A124" s="4"/>
+      <c r="B124" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="C124" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="D124" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E124" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F124" s="6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A125" s="4"/>
+      <c r="B125" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C125" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="D125" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E125" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F125" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A126" s="4"/>
+      <c r="B126" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C126" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="D126" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E126" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F126" s="6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A127" s="4"/>
+      <c r="B127" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="C127" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="D127" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E127" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F127" s="6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A128" s="4"/>
+      <c r="B128" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="C128" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="D128" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="E128" s="8"/>
+      <c r="F128" s="6" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A129" s="4"/>
+      <c r="B129" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C129" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="D129" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E129" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F129" s="6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A130" s="4"/>
+      <c r="B130" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C130" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="D130" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E130" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F130" s="6" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A131" s="4"/>
+      <c r="B131" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C131" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="D131" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E131" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="F131" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A132" s="4"/>
+      <c r="B132" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C132" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="D132" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E132" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F132" s="6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A133" s="4"/>
+      <c r="B133" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="C133" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="D133" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E133" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F133" s="6" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A134" s="4"/>
+      <c r="B134" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="C134" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="D134" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E134" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F134" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A104:A108"/>
+    <mergeCell ref="A109:A134"/>
+    <mergeCell ref="A88:A90"/>
+    <mergeCell ref="A91:A94"/>
+    <mergeCell ref="A95:A98"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="A66:A84"/>
+    <mergeCell ref="A47:A65"/>
+    <mergeCell ref="A85:A87"/>
+    <mergeCell ref="A25:A37"/>
+    <mergeCell ref="A38:A46"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A24"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="256" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>